<commit_message>
Added steps 1-4(description,images) and code
</commit_message>
<xml_diff>
--- a/DIY Mastersheet.xlsx
+++ b/DIY Mastersheet.xlsx
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
PIR Sensor and Index.html
</commit_message>
<xml_diff>
--- a/DIY Mastersheet.xlsx
+++ b/DIY Mastersheet.xlsx
@@ -1,15 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Members" sheetId="1" r:id="rId1"/>
     <sheet name="Project List" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Project List'!$A$1:$F$25</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -309,7 +312,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -344,7 +347,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -521,7 +524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -535,9 +538,9 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -595,23 +598,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.44140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -631,7 +635,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="43.8" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -639,7 +643,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -647,7 +651,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -658,7 +662,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="72.599999999999994" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -666,7 +670,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>43</v>
       </c>
@@ -677,7 +681,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -685,7 +689,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -693,7 +697,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -701,7 +705,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -709,7 +713,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -717,7 +721,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
@@ -728,7 +732,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -736,7 +740,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
@@ -744,7 +748,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -752,7 +756,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -760,7 +764,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
@@ -768,7 +772,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>28</v>
       </c>
@@ -776,7 +780,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>42</v>
       </c>
@@ -793,37 +797,44 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F25">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B26">
       <formula1>"Gautam, Pallavi, Rizwan, Sairam, Maria"</formula1>

</xml_diff>

<commit_message>
Created folders under diy
</commit_message>
<xml_diff>
--- a/DIY Mastersheet.xlsx
+++ b/DIY Mastersheet.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Members" sheetId="1" r:id="rId1"/>
     <sheet name="Project List" sheetId="2" r:id="rId2"/>
+    <sheet name="Common components" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Project List'!$A$1:$F$25</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
   <si>
     <t>Member Name</t>
   </si>
@@ -74,9 +75,6 @@
     <t>Water meter which shows both flow of water as well as volume</t>
   </si>
   <si>
-    <t>Detection of water in drywaste bin by use of moisture/rain sensor and it beeps if there is water detected</t>
-  </si>
-  <si>
     <t>Vermicomposting moisture indicator</t>
   </si>
   <si>
@@ -92,9 +90,6 @@
     <t>Smart drip irrigation</t>
   </si>
   <si>
-    <t>Waste Bin rewarder</t>
-  </si>
-  <si>
     <t>Energy saver from Lamp posts</t>
   </si>
   <si>
@@ -113,9 +108,6 @@
     <t>Water Alert Detector</t>
   </si>
   <si>
-    <t>Automtic lights and fans</t>
-  </si>
-  <si>
     <t>Bluetooth control lights</t>
   </si>
   <si>
@@ -134,9 +126,6 @@
     <t>Area (WWES)</t>
   </si>
   <si>
-    <t>Issue (What does it solve?)</t>
-  </si>
-  <si>
     <t>Waste</t>
   </si>
   <si>
@@ -158,14 +147,59 @@
     <t>Automatic fan switch on based on humidity and temperature</t>
   </si>
   <si>
-    <t>Boxing pending</t>
+    <t>Here</t>
+  </si>
+  <si>
+    <t>Link to master</t>
+  </si>
+  <si>
+    <t>Breadboard</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Soil moisture sensor</t>
+  </si>
+  <si>
+    <t>DHT</t>
+  </si>
+  <si>
+    <t>Components</t>
+  </si>
+  <si>
+    <t>Relay</t>
+  </si>
+  <si>
+    <t>LCD</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Working</t>
+  </si>
+  <si>
+    <t>Automatic lights and fans</t>
+  </si>
+  <si>
+    <t>Dry waste bin- beeps if wet</t>
+  </si>
+  <si>
+    <t>Dry waste bin- display using LCD if wet</t>
+  </si>
+  <si>
+    <t>Images, video pending</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,8 +232,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +251,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -237,10 +285,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -252,11 +301,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -601,11 +658,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +675,7 @@
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -632,222 +688,347 @@
       <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
+      <c r="E1" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="G1" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
       <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
       <c r="E6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="E12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D19" s="2">
         <v>43313</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:F25">
-    <filterColumn colId="1">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B26">
       <formula1>"Gautam, Pallavi, Rizwan, Sairam, Maria"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1"/>
+    <hyperlink ref="F5" r:id="rId2"/>
+    <hyperlink ref="F19" r:id="rId3"/>
+    <hyperlink ref="F11" r:id="rId4"/>
+    <hyperlink ref="F18" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="B3" r:id="rId5"/>
+    <hyperlink ref="B5" r:id="rId6"/>
+    <hyperlink ref="B6" r:id="rId7"/>
+    <hyperlink ref="C6" r:id="rId8"/>
+    <hyperlink ref="C7" r:id="rId9"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated energy>>temperature and humidity controlled fan
</commit_message>
<xml_diff>
--- a/DIY Mastersheet.xlsx
+++ b/DIY Mastersheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
   <si>
     <t>Member Name</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Moisture based smart irrigation</t>
   </si>
   <si>
-    <t>Automatic fan switch on based on humidity and temperature</t>
-  </si>
-  <si>
     <t>Here</t>
   </si>
   <si>
@@ -196,6 +193,12 @@
   </si>
   <si>
     <t>Smart taps</t>
+  </si>
+  <si>
+    <t>Temperature and humidity controlled fan</t>
+  </si>
+  <si>
+    <t>Boxing image, video pending</t>
   </si>
 </sst>
 </file>
@@ -244,7 +247,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,6 +263,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,7 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -315,6 +324,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -667,7 +679,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +710,7 @@
         <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1">
         <v>15</v>
@@ -728,30 +740,30 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>36</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -762,30 +774,30 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
         <v>30</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
         <v>32</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -796,13 +808,13 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
         <v>32</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -816,7 +828,7 @@
         <v>32</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -829,19 +841,19 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
         <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
       </c>
       <c r="E11" t="s">
         <v>30</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -852,13 +864,13 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
         <v>33</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -869,13 +881,13 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -896,19 +908,19 @@
     </row>
     <row r="16" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s">
         <v>32</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -921,19 +933,19 @@
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
         <v>30</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -953,24 +965,24 @@
         <v>32</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" t="s">
         <v>33</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -980,19 +992,19 @@
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" t="s">
         <v>32</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1007,19 +1019,19 @@
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E25" t="s">
         <v>30</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1070,74 +1082,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>